<commit_message>
Rechtschreibfehler + Regelbetrieb Definition
</commit_message>
<xml_diff>
--- a/Glossar.xlsx
+++ b/Glossar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Desktop\HAW\Bachelorprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9161C982-FFE0-4DA4-AE48-7D2F2A944714}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D834A622-E2F1-48B7-9D12-FA5F0F9F4D99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{E1040B1C-CE54-4464-8256-39420C39D080}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{E1040B1C-CE54-4464-8256-39420C39D080}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>Papierkneuel</t>
-  </si>
-  <si>
     <t>Werkzeugaufsätze</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>Zigarettenfilter, die aus Cellulose-Acetat bestehen.</t>
   </si>
   <si>
-    <t>1 ½ Stunden ununterbrochen in einen Job tätig.</t>
-  </si>
-  <si>
     <t>Rahmenbedingungen der Detektion</t>
   </si>
   <si>
@@ -177,10 +171,16 @@
     <t>- Reichweite &gt; 50mm</t>
   </si>
   <si>
-    <t>Piken</t>
-  </si>
-  <si>
-    <t>Unmittelbar aufeinanderfolgende Ab-Aufwärtsbewegung zur Aufnahme von Zigarettenstummel</t>
+    <t>Papierknäuel</t>
+  </si>
+  <si>
+    <t>½ Stunde ununterbrochen in einen Job tätig.</t>
+  </si>
+  <si>
+    <t>Pieken</t>
+  </si>
+  <si>
+    <t>Unmittelbar aufeinanderfolgende Ab- und Aufwärtsbewegung zur Aufnahme von Zigarettenstummel</t>
   </si>
 </sst>
 </file>
@@ -580,17 +580,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFE7F6D-8032-4E4D-942A-E35A214CDFA1}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="88.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.59765625" customWidth="1"/>
+    <col min="2" max="2" width="88.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -598,143 +598,143 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="B17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>48</v>
       </c>
@@ -742,72 +742,72 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
       <c r="B23" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
       <c r="B25" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
       <c r="B29" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
       <c r="B30" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>